<commit_message>
added coolant temp to the code doc
</commit_message>
<xml_diff>
--- a/RX8CanBus20-05-2020_Will_additions.xlsx
+++ b/RX8CanBus20-05-2020_Will_additions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livemdxac-my.sharepoint.com/personal/w_davis_mdx_ac_uk/Documents/Inventions/IsaacRX8/MazdaRX8Arduino-master/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\OneDrive - Middlesex University\Inventions\IsaacRX8\MazdaRX8TelemetryScreen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="111">
   <si>
     <t>CAN ID</t>
   </si>
@@ -359,13 +359,16 @@
   </si>
   <si>
     <t>*Will's additions from the chinese arduino script</t>
+  </si>
+  <si>
+    <t>Coolant Temp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -400,6 +403,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -443,7 +452,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -468,6 +477,8 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="3"/>
@@ -788,7 +799,7 @@
   <dimension ref="A1:S49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1533,8 +1544,8 @@
         <v>55</v>
       </c>
       <c r="B34" s="2"/>
-      <c r="C34" s="2" t="s">
-        <v>60</v>
+      <c r="C34" s="19" t="s">
+        <v>110</v>
       </c>
       <c r="D34" s="9">
         <v>8</v>
@@ -1548,7 +1559,7 @@
       <c r="G34" s="9">
         <v>191</v>
       </c>
-      <c r="H34" s="9">
+      <c r="H34" s="18">
         <v>127</v>
       </c>
       <c r="I34" s="9">
@@ -1963,6 +1974,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010042EF5B5FED3C1B46A089224F4BBBC839" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c677d527518b1c4a0cc40f6d2906d1f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cc544dc1-3c9d-46e1-9f0b-6c4877d0412d" xmlns:ns4="a8ad2cf7-3990-4386-aca2-65ff249e7667" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8eb838a1d1421da135dd40b578a319ee" ns3:_="" ns4:_="">
     <xsd:import namespace="cc544dc1-3c9d-46e1-9f0b-6c4877d0412d"/>
@@ -2191,22 +2217,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{659B407F-4646-43EC-83C5-F0F687CFCA8D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="cc544dc1-3c9d-46e1-9f0b-6c4877d0412d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a8ad2cf7-3990-4386-aca2-65ff249e7667"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A11F17F8-1594-43D1-B0AB-001D9004130F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07094125-D120-4FF9-B0F0-2920827FE411}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2223,29 +2259,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A11F17F8-1594-43D1-B0AB-001D9004130F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{659B407F-4646-43EC-83C5-F0F687CFCA8D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="a8ad2cf7-3990-4386-aca2-65ff249e7667"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="cc544dc1-3c9d-46e1-9f0b-6c4877d0412d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>